<commit_message>
FPP file was checked and corrected
</commit_message>
<xml_diff>
--- a/RELEASE/VMRAM/VMRAM-FPP.xlsx
+++ b/RELEASE/VMRAM/VMRAM-FPP.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\Desktop\GRUPOVMRAM\RELEASE\VMRAM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9390"/>
   </bookViews>
@@ -81,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,8 +277,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -290,6 +293,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,60 +354,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,7 +409,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="3 Imagen"/>
+        <xdr:cNvPr id="4" name="3 Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -690,7 +705,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,24 +715,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32:J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="3.453125" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -730,7 +745,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -743,35 +758,35 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -784,50 +799,50 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="4"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="33"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -840,7 +855,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="26" t="s">
         <v>9</v>
@@ -857,11 +872,11 @@
       <c r="J10" s="6"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -870,7 +885,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="26" t="s">
         <v>0</v>
@@ -885,39 +900,39 @@
       <c r="J12" s="23"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -926,11 +941,11 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -939,7 +954,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="26" t="s">
         <v>1</v>
@@ -954,7 +969,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -967,23 +982,23 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="8" t="s">
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="41" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="38" t="s">
@@ -992,9 +1007,9 @@
       <c r="J19" s="39"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="10">
+      <c r="B20" s="8">
         <v>1</v>
       </c>
       <c r="C20" s="23"/>
@@ -1002,14 +1017,14 @@
       <c r="E20" s="23"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="41"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <v>2</v>
       </c>
       <c r="C21" s="23"/>
@@ -1017,41 +1032,41 @@
       <c r="E21" s="23"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="41"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="8" t="s">
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H23" s="41" t="s">
         <v>5</v>
       </c>
       <c r="I23" s="38" t="s">
@@ -1060,9 +1075,9 @@
       <c r="J23" s="39"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="12">
+      <c r="B24" s="10">
         <v>1</v>
       </c>
       <c r="C24" s="23"/>
@@ -1070,14 +1085,14 @@
       <c r="E24" s="23"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="41"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <v>2</v>
       </c>
       <c r="C25" s="23"/>
@@ -1085,41 +1100,41 @@
       <c r="E25" s="23"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="41"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="8" t="s">
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="41" t="s">
         <v>5</v>
       </c>
       <c r="I27" s="38" t="s">
@@ -1128,9 +1143,9 @@
       <c r="J27" s="39"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <v>1</v>
       </c>
       <c r="C28" s="23"/>
@@ -1138,14 +1153,14 @@
       <c r="E28" s="23"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="41"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
-      <c r="B29" s="12">
+      <c r="B29" s="10">
         <v>2</v>
       </c>
       <c r="C29" s="23"/>
@@ -1153,12 +1168,12 @@
       <c r="E29" s="23"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1171,23 +1186,23 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="8" t="s">
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="41" t="s">
         <v>5</v>
       </c>
       <c r="I31" s="38" t="s">
@@ -1196,9 +1211,9 @@
       <c r="J31" s="39"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="12">
+      <c r="B32" s="10">
         <v>1</v>
       </c>
       <c r="C32" s="23"/>
@@ -1206,14 +1221,14 @@
       <c r="E32" s="23"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="41"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="25"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="12">
+      <c r="B33" s="10">
         <v>2</v>
       </c>
       <c r="C33" s="23"/>
@@ -1221,12 +1236,12 @@
       <c r="E33" s="23"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="41"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="25"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1239,7 +1254,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1252,12 +1267,12 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="27"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1267,7 +1282,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
@@ -1280,7 +1295,7 @@
       <c r="J37" s="23"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="23"/>
       <c r="C38" s="23"/>
@@ -1293,7 +1308,7 @@
       <c r="J38" s="23"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
@@ -1306,7 +1321,7 @@
       <c r="J39" s="23"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
@@ -1319,7 +1334,7 @@
       <c r="J40" s="23"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1332,7 +1347,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1345,7 +1360,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1358,24 +1373,24 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="22" t="s">
+      <c r="H44" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="I44" s="22"/>
+      <c r="I44" s="34"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1388,7 +1403,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1401,7 +1416,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1416,20 +1431,17 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="E3:J4"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="B37:J40"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
@@ -1443,17 +1455,20 @@
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="I24:J24"/>
-    <mergeCell ref="E3:J4"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="I32:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>